<commit_message>
new BOM after crafty help
</commit_message>
<xml_diff>
--- a/electronics/hapy2.5/PE_BrainRisebox.xlsx
+++ b/electronics/hapy2.5/PE_BrainRisebox.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="306">
   <si>
     <t>Repere topographique</t>
   </si>
@@ -88,7 +88,7 @@
     <t>http://fr.rs-online.com/web/p/condensateurs-ceramique-multicouche/7900594/?searchTerm=GRM31CC8YA106KA12L&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D6672266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D313326736E3D592673743D4D414E5F504152545F4E554D4245522677633D424F5448267573743D47524D333143433859413130364B4131324C26</t>
   </si>
   <si>
-    <t>C5,C13</t>
+    <t>C5,C13,C21,C22</t>
   </si>
   <si>
     <t>Condensateur 0.1uF C_0402</t>
@@ -214,28 +214,31 @@
     <t>D5</t>
   </si>
   <si>
-    <t>Diode Simple Zener SMB</t>
-  </si>
-  <si>
-    <t>1SMB5935BT3G</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/on-semiconductor/1smb5935bt3g/diode-zener-3w-27v/dp/1431177</t>
+    <t>TRANSIL</t>
+  </si>
+  <si>
+    <t>SMBJ26A/CA</t>
+  </si>
+  <si>
+    <t>1749318</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/stmicroelectronics/smbj26a-tr/transil-600w-26v-unidir-smb/dp/1749318</t>
   </si>
   <si>
     <t>D7</t>
   </si>
   <si>
-    <t>Diode Zener SOD43</t>
-  </si>
-  <si>
     <t>FAIRCHILD SEMICONDUCTOR</t>
   </si>
   <si>
-    <t>MMSZ4702</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/fairchild-semiconductor/mmsz4702/diode-zener-0-5w-15v-sod-123/dp/1700853</t>
+    <t>SMBJ15A/CA</t>
+  </si>
+  <si>
+    <t>9886117</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/stmicroelectronics/smbj15a-tr/diode-de-suppression-600w-15v/dp/9886117</t>
   </si>
   <si>
     <t>D8,D15</t>
@@ -286,7 +289,7 @@
     <t>http://fr.farnell.com/kingbright/kpt-1608yc/led-jaune-0603-cms/dp/2099227?ost=KPT-1608YC</t>
   </si>
   <si>
-    <t>D14</t>
+    <t>D14, D17</t>
   </si>
   <si>
     <t>Diode Zener SOD123</t>
@@ -361,162 +364,159 @@
     <t>http://fr.rs-online.com/web/p/transistors-mosfet/6710312/</t>
   </si>
   <si>
-    <t>Quel ampérage, y'a moins cher sinon</t>
-  </si>
-  <si>
     <t>Q2</t>
   </si>
   <si>
-    <t>MOSFET Canal N SOT23 500mA</t>
+    <t>MOSFET Canal N SOT23 2.2A</t>
+  </si>
+  <si>
+    <t>FDN337N</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/fairchild-semiconductor/fdn337n/transistor-mosfet-n-sot-23/dp/9845356</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Transistor de puissance PNP 1,5A</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>BD140</t>
+  </si>
+  <si>
+    <t>314-1817</t>
+  </si>
+  <si>
+    <t>http://fr.rs-online.com/web/p/transistors-bipolaires/3141817/</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>MOSFET Canal P SOT 23 FET</t>
+  </si>
+  <si>
+    <t>INFINEON</t>
+  </si>
+  <si>
+    <t>BSS84P-H6327</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/infineon/bss84p-h6327/transistor-mosfet-canal-p-boitier/dp/1056526</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Resistance CMS 24.3K 1% 0603</t>
+  </si>
+  <si>
+    <t>VISHAY DRALORIC</t>
+  </si>
+  <si>
+    <t>CRCW060324K3FKEA</t>
+  </si>
+  <si>
+    <t>2138446</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/vishay-draloric/crcw060324k3fkea/resistance-0603-24k3-1/dp/2138446</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Resistance CMS 11.5K 1% 0603</t>
+  </si>
+  <si>
+    <t>PANASONIC ELECTRONIC COMPONENTS</t>
+  </si>
+  <si>
+    <t>ERJP03F1152V</t>
+  </si>
+  <si>
+    <t>2311932RL</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/panasonic-electronic-components/erjp03f1152v/resistance-erjp-11-5k-0603-0-2w/dp/2311932RL</t>
+  </si>
+  <si>
+    <t>R4, R11</t>
+  </si>
+  <si>
+    <t>Resistance CMS 43.2K 1% 0603</t>
+  </si>
+  <si>
+    <t>CRCW060343K2FKEA</t>
+  </si>
+  <si>
+    <t>1469810</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/vishay-draloric/crcw060343k2fkea/resistance-0603-43k2-1/dp/1469810</t>
+  </si>
+  <si>
+    <t>R5, R12</t>
+  </si>
+  <si>
+    <t>Resistance CMS 143K 1% 0603</t>
+  </si>
+  <si>
+    <t>CRCW0603143KFKEA</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/panasonic-electronic-components/erj3ekf1433v/resist-couche-epaisse-143k-100mw/dp/2303238</t>
+  </si>
+  <si>
+    <t>R6, R13</t>
+  </si>
+  <si>
+    <t>Resistance CMS 3.74k 1% 0603</t>
+  </si>
+  <si>
+    <t>VISHAY DALE </t>
+  </si>
+  <si>
+    <t>CRCW06033K74FKEA</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/vishay-dale/crcw06033k74fkea/thick-film-resistor-3-74kohm-100mw/dp/1151910</t>
+  </si>
+  <si>
+    <t>R7, R14</t>
+  </si>
+  <si>
+    <t>Resistance CMS 51.1ohm 1% 0603</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>ERA3AEB51R1V</t>
+  </si>
+  <si>
+    <t>708-7041</t>
+  </si>
+  <si>
+    <t>http://fr.rs-online.com/web/p/resistances-cms/7087041/</t>
+  </si>
+  <si>
+    <t>C'est quoi la résstenace des 55.1 ohm ou kOhmk ?</t>
+  </si>
+  <si>
+    <t>R8, R15</t>
+  </si>
+  <si>
+    <t>Resistance CMS 100k 1% 0603</t>
   </si>
   <si>
     <t>Vishay</t>
   </si>
   <si>
-    <t>2N7002K-T1-E3</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/vishay-siliconix/2n7002k-t1-e3/n-channel-mosfet-60v-0-5a-sot/dp/1837251?ost=2N7002&amp;categoryId=700000043507</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Transistor de puissance PNP 1,5A</t>
-  </si>
-  <si>
-    <t>STMicroelectronics</t>
-  </si>
-  <si>
-    <t>BD140</t>
-  </si>
-  <si>
-    <t>314-1817</t>
-  </si>
-  <si>
-    <t>http://fr.rs-online.com/web/p/transistors-bipolaires/3141817/</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>MOSFET Canal P SOT 23 FET</t>
-  </si>
-  <si>
-    <t>INFINEON</t>
-  </si>
-  <si>
-    <t>BSS84P-H6327</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/infineon/bss84p-h6327/transistor-mosfet-canal-p-boitier/dp/1056526</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>Resistance CMS 24.3K 1% 0603</t>
-  </si>
-  <si>
-    <t>VISHAY DRALORIC</t>
-  </si>
-  <si>
-    <t>CRCW060324K3FKEA</t>
-  </si>
-  <si>
-    <t>2138446</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/vishay-draloric/crcw060324k3fkea/resistance-0603-24k3-1/dp/2138446</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>Resistance CMS 11.5K 1% 0603</t>
-  </si>
-  <si>
-    <t>PANASONIC ELECTRONIC COMPONENTS</t>
-  </si>
-  <si>
-    <t>ERJP03F1152V</t>
-  </si>
-  <si>
-    <t>2311932RL</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/panasonic-electronic-components/erjp03f1152v/resistance-erjp-11-5k-0603-0-2w/dp/2311932RL</t>
-  </si>
-  <si>
-    <t>R4, R11</t>
-  </si>
-  <si>
-    <t>Resistance CMS 43.2K 1% 0603</t>
-  </si>
-  <si>
-    <t>CRCW060343K2FKEA</t>
-  </si>
-  <si>
-    <t>1469810</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/vishay-draloric/crcw060343k2fkea/resistance-0603-43k2-1/dp/1469810</t>
-  </si>
-  <si>
-    <t>R5, R12</t>
-  </si>
-  <si>
-    <t>Resistance CMS 143K 1% 0603</t>
-  </si>
-  <si>
-    <t>CRCW0603143KFKEA</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/panasonic-electronic-components/erj3ekf1433v/resist-couche-epaisse-143k-100mw/dp/2303238</t>
-  </si>
-  <si>
-    <t>R6, R13</t>
-  </si>
-  <si>
-    <t>Resistance CMS 3.74k 1% 0603</t>
-  </si>
-  <si>
-    <t>VISHAY DALE </t>
-  </si>
-  <si>
-    <t>CRCW06033K74FKEA</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/vishay-dale/crcw06033k74fkea/thick-film-resistor-3-74kohm-100mw/dp/1151910</t>
-  </si>
-  <si>
-    <t>R7, R14</t>
-  </si>
-  <si>
-    <t>Resistance CMS 51.1ohm 1% 0603</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
-    <t>ERA3AEB51R1V</t>
-  </si>
-  <si>
-    <t>708-7041</t>
-  </si>
-  <si>
-    <t>http://fr.rs-online.com/web/p/resistances-cms/7087041/</t>
-  </si>
-  <si>
-    <t>C'est quoi la résstenace des 55.1 ohm ou kOhmk ?</t>
-  </si>
-  <si>
-    <t>R8, R15</t>
-  </si>
-  <si>
-    <t>Resistance CMS 100k 1% 0603</t>
-  </si>
-  <si>
     <t>CRCW0603100KFKEAHP</t>
   </si>
   <si>
@@ -571,7 +571,7 @@
     <t>http://fr.rs-online.com/web/p/resistances-cms/6790419/</t>
   </si>
   <si>
-    <t>R18,R35,R42,R45,R51</t>
+    <t>R18,R35,R42,R45,R51,R57,R54</t>
   </si>
   <si>
     <t>Resistance CMS 100 1% 0603</t>
@@ -589,7 +589,7 @@
     <t>http://fr.rs-online.com/web/p/resistances-cms/2132143/</t>
   </si>
   <si>
-    <t>R19,R22,R25,R26,R28,R31,R33,R34,R36,R52</t>
+    <t>R22,R25,R26,R28,R31,R33,R34,R36</t>
   </si>
   <si>
     <t>Resistance CMS 1k 1% 0603</t>
@@ -634,7 +634,7 @@
     <t>http://fr.rs-online.com/web/p/resistances-cms/6789926/</t>
   </si>
   <si>
-    <t>R23,R24,R29,R30,R40,R43,R48</t>
+    <t>R19, R23,R24,R29,R30,R40,R43,R48,R56,R55,R52</t>
   </si>
   <si>
     <t>Resistance CMS 10k 1% 0603</t>
@@ -892,16 +892,16 @@
     <t>R41</t>
   </si>
   <si>
-    <t>Résistance 56 ohms 1% 0805</t>
-  </si>
-  <si>
-    <t>CRCW080556R0FKEA</t>
-  </si>
-  <si>
-    <t>679-1557</t>
-  </si>
-  <si>
-    <t>http://fr.rs-online.com/web/p/resistances-cms/6791557/</t>
+    <t>Résistance 56 ohms 1% 1206</t>
+  </si>
+  <si>
+    <t>CRCW120656R0FKEAHP</t>
+  </si>
+  <si>
+    <t>812-1922</t>
+  </si>
+  <si>
+    <t>http://fr.rs-online.com/web/p/resistances-cms/8121922/</t>
   </si>
   <si>
     <t>R44</t>
@@ -1024,7 +1024,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1045,24 +1045,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1084,22 +1076,22 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I49" activeCellId="0" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.30612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.71428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.3214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.1785714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.87755102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="179.301020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="25.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.35714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.12755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.9234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.71428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="176.831632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="24.8571428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,10 +1134,10 @@
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1175,7 +1167,7 @@
       <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1194,7 +1186,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -1202,7 +1194,7 @@
       <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1229,7 +1221,7 @@
       <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="3" t="n">
@@ -1256,7 +1248,7 @@
       <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="3" t="n">
@@ -1283,7 +1275,7 @@
       <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G7" s="3" t="n">
@@ -1310,10 +1302,10 @@
       <c r="E8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>46</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -1340,7 +1332,7 @@
       <c r="E9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>52</v>
       </c>
       <c r="G9" s="3" t="n">
@@ -1367,7 +1359,7 @@
       <c r="E10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>57</v>
       </c>
       <c r="G10" s="3" t="n">
@@ -1394,7 +1386,7 @@
       <c r="E11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>62</v>
       </c>
       <c r="G11" s="3" t="n">
@@ -1421,62 +1413,62 @@
       <c r="E12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="3" t="n">
-        <v>1431177</v>
+      <c r="G12" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="3" t="n">
-        <v>1700853</v>
+      <c r="G13" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="5" t="s">
         <v>76</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="G14" s="3" t="n">
         <v>2426211</v>
@@ -1485,55 +1477,55 @@
         <v>28</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="F15" s="3" t="s">
         <v>82</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="G16" s="3" t="n">
         <v>2099227</v>
@@ -1542,28 +1534,28 @@
         <v>28</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="3" t="s">
         <v>57</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>28</v>
@@ -1575,73 +1567,73 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F18" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="F18" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G18" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="5" t="s">
         <v>101</v>
       </c>
+      <c r="F19" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G19" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="5" t="s">
         <v>107</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="G20" s="3" t="n">
         <v>3417657</v>
@@ -1650,38 +1642,36 @@
         <v>28</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>110</v>
+      <c r="D21" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>111</v>
+      <c r="F21" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J21" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
@@ -1691,69 +1681,69 @@
       <c r="C22" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="n">
+        <v>9845356</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="G22" s="6" t="n">
-        <v>1837251</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="J22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>14</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="G24" s="3" t="n">
         <v>1056526</v>
@@ -1762,106 +1752,106 @@
         <v>28</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="H27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
       <c r="B28" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="G28" s="3" t="n">
         <v>2303238</v>
@@ -1870,25 +1860,25 @@
         <v>28</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="G29" s="3" t="n">
         <v>1151910</v>
@@ -1897,57 +1887,57 @@
         <v>28</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>14</v>
       </c>
       <c r="I30" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="5" t="s">
         <v>167</v>
       </c>
       <c r="H31" s="0" t="s">
@@ -1968,12 +1958,12 @@
         <v>170</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="5" t="s">
         <v>172</v>
       </c>
       <c r="H32" s="0" t="s">
@@ -1994,12 +1984,12 @@
         <v>175</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F33" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G33" s="5" t="s">
         <v>177</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -2022,10 +2012,10 @@
       <c r="E34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="5" t="s">
         <v>182</v>
       </c>
       <c r="H34" s="2" t="s">
@@ -2040,7 +2030,7 @@
         <v>184</v>
       </c>
       <c r="C35" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>185</v>
@@ -2048,10 +2038,10 @@
       <c r="E35" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="G35" s="5" t="s">
         <v>188</v>
       </c>
       <c r="H35" s="2" t="s">
@@ -2062,11 +2052,11 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>190</v>
       </c>
       <c r="C36" s="3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>191</v>
@@ -2074,10 +2064,10 @@
       <c r="E36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G36" s="5" t="s">
         <v>193</v>
       </c>
       <c r="H36" s="2" t="s">
@@ -2088,7 +2078,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>195</v>
       </c>
       <c r="C37" s="3" t="n">
@@ -2100,10 +2090,10 @@
       <c r="E37" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G37" s="5" t="s">
         <v>198</v>
       </c>
       <c r="H37" s="2" t="s">
@@ -2114,7 +2104,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>200</v>
       </c>
       <c r="C38" s="3" t="n">
@@ -2124,12 +2114,12 @@
         <v>201</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F38" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="G38" s="5" t="s">
         <v>203</v>
       </c>
       <c r="H38" s="2" t="s">
@@ -2144,7 +2134,7 @@
         <v>205</v>
       </c>
       <c r="C39" s="3" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>206</v>
@@ -2152,10 +2142,10 @@
       <c r="E39" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G39" s="5" t="s">
         <v>209</v>
       </c>
       <c r="H39" s="2" t="s">
@@ -2178,10 +2168,10 @@
       <c r="E40" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G40" s="5" t="s">
         <v>214</v>
       </c>
       <c r="H40" s="2" t="s">
@@ -2204,10 +2194,10 @@
       <c r="E41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" s="5" t="s">
         <v>218</v>
       </c>
       <c r="H41" s="2" t="s">
@@ -2230,10 +2220,10 @@
       <c r="E42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G42" s="5" t="s">
         <v>223</v>
       </c>
       <c r="H42" s="2" t="s">
@@ -2256,10 +2246,10 @@
       <c r="E43" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G43" s="5" t="s">
         <v>228</v>
       </c>
       <c r="H43" s="2" t="s">
@@ -2282,10 +2272,10 @@
       <c r="E44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="G44" s="6" t="s">
+      <c r="G44" s="5" t="s">
         <v>233</v>
       </c>
       <c r="H44" s="2" t="s">
@@ -2302,16 +2292,16 @@
       <c r="C45" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="6" t="s">
         <v>236</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G45" s="5" t="s">
         <v>239</v>
       </c>
       <c r="H45" s="2" t="s">
@@ -2334,16 +2324,16 @@
       <c r="E46" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="G46" s="5" t="s">
         <v>244</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I46" s="6" t="s">
+      <c r="I46" s="5" t="s">
         <v>245</v>
       </c>
     </row>
@@ -2360,10 +2350,10 @@
       <c r="E47" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="G47" s="5" t="s">
         <v>250</v>
       </c>
       <c r="H47" s="2" t="s">
@@ -2386,10 +2376,10 @@
       <c r="E48" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F48" s="5" t="n">
+      <c r="F48" s="3" t="n">
         <v>1725656</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="G48" s="5" t="s">
         <v>255</v>
       </c>
       <c r="H48" s="2" t="s">
@@ -2412,10 +2402,10 @@
       <c r="E49" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F49" s="5" t="n">
+      <c r="F49" s="3" t="n">
         <v>1725669</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="G49" s="5" t="s">
         <v>259</v>
       </c>
       <c r="H49" s="2" t="s">
@@ -2438,10 +2428,10 @@
       <c r="E50" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="G50" s="5" t="s">
         <v>264</v>
       </c>
       <c r="H50" s="2" t="s">
@@ -2464,10 +2454,10 @@
       <c r="E51" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F51" s="5" t="n">
+      <c r="F51" s="3" t="n">
         <v>1725698</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="G51" s="5" t="s">
         <v>269</v>
       </c>
       <c r="H51" s="2" t="s">
@@ -2490,10 +2480,10 @@
       <c r="E52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="G52" s="6" t="s">
+      <c r="G52" s="5" t="s">
         <v>274</v>
       </c>
       <c r="H52" s="2" t="s">
@@ -2516,10 +2506,10 @@
       <c r="E53" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G53" s="6" t="n">
+      <c r="G53" s="5" t="n">
         <v>2346999</v>
       </c>
       <c r="H53" s="2" t="s">
@@ -2542,10 +2532,10 @@
       <c r="E54" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="G54" s="6" t="s">
+      <c r="G54" s="5" t="s">
         <v>284</v>
       </c>
       <c r="H54" s="2" t="s">
@@ -2562,14 +2552,14 @@
       <c r="C55" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="6" t="s">
         <v>287</v>
       </c>
       <c r="E55" s="3"/>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="G55" s="6" t="n">
+      <c r="G55" s="5" t="n">
         <v>2215311</v>
       </c>
       <c r="H55" s="2" t="s">
@@ -2590,12 +2580,12 @@
         <v>291</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="G56" s="5" t="s">
         <v>293</v>
       </c>
       <c r="H56" s="2" t="s">
@@ -2618,10 +2608,10 @@
       <c r="E57" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G57" s="5" t="s">
         <v>298</v>
       </c>
       <c r="H57" s="2" t="s">
@@ -2644,10 +2634,10 @@
       <c r="E58" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="G58" s="6" t="s">
+      <c r="G58" s="5" t="s">
         <v>304</v>
       </c>
       <c r="H58" s="2" t="s">
@@ -2687,57 +2677,58 @@
     <hyperlink ref="G4" r:id="rId1" display="2113067"/>
     <hyperlink ref="F8" r:id="rId2" display="12061C104JAT2A"/>
     <hyperlink ref="G8" r:id="rId3" display="2332842"/>
-    <hyperlink ref="E15" r:id="rId4" display="NXP"/>
-    <hyperlink ref="F17" r:id="rId5" display="MMSZ4678T1G"/>
-    <hyperlink ref="G17" r:id="rId6" display="1459115"/>
-    <hyperlink ref="G18" r:id="rId7" display="9943641"/>
-    <hyperlink ref="G19" r:id="rId8" display="2289092"/>
-    <hyperlink ref="E20" r:id="rId9" display=" TE CONNECTIVITY / AMP"/>
-    <hyperlink ref="E23" r:id="rId10" display="STMicroelectronics"/>
-    <hyperlink ref="G23" r:id="rId11" display="314-1817"/>
-    <hyperlink ref="F25" r:id="rId12" display="CRCW060324K3FKEA"/>
-    <hyperlink ref="G25" r:id="rId13" display="2138446"/>
-    <hyperlink ref="F26" r:id="rId14" display="ERJP03F1152V"/>
-    <hyperlink ref="G26" r:id="rId15" display="2311932RL"/>
-    <hyperlink ref="F27" r:id="rId16" display="CRCW060343K2FKEA"/>
-    <hyperlink ref="G27" r:id="rId17" display="1469810"/>
-    <hyperlink ref="F28" r:id="rId18" display="CRCW0603143KFKEA"/>
-    <hyperlink ref="E30" r:id="rId19" display="Panasonic"/>
-    <hyperlink ref="E31" r:id="rId20" display="Vishay"/>
-    <hyperlink ref="G31" r:id="rId21" display="820-6745"/>
-    <hyperlink ref="E32" r:id="rId22" display="Vishay"/>
-    <hyperlink ref="G34" r:id="rId23" display="679-0419"/>
-    <hyperlink ref="G35" r:id="rId24" display="213-2143"/>
-    <hyperlink ref="G36" r:id="rId25" display="213-2266"/>
-    <hyperlink ref="E38" r:id="rId26" display="Vishay"/>
-    <hyperlink ref="G38" r:id="rId27" display="678-9926"/>
-    <hyperlink ref="G39" r:id="rId28" display="740-8805"/>
-    <hyperlink ref="G40" r:id="rId29" display="740-8877"/>
-    <hyperlink ref="G41" r:id="rId30" display="679-0251"/>
-    <hyperlink ref="G42" r:id="rId31" display="679-0689"/>
-    <hyperlink ref="G43" r:id="rId32" display="678-9960"/>
-    <hyperlink ref="G44" r:id="rId33" display="678-9822"/>
-    <hyperlink ref="E45" r:id="rId34" display="KNITTER-SWITCH"/>
-    <hyperlink ref="E46" r:id="rId35" display="TE Connectivity"/>
-    <hyperlink ref="I46" r:id="rId36" display="http://fr.rs-online.com/web/p/embases-de-circuit-imprime/4958486/"/>
-    <hyperlink ref="F47" r:id="rId37" display="LM317MDCYRG3"/>
-    <hyperlink ref="G47" r:id="rId38" display="1640686"/>
-    <hyperlink ref="E48" r:id="rId39" display="Phoenix Contact"/>
-    <hyperlink ref="E49" r:id="rId40" display="Phoenix Contact"/>
-    <hyperlink ref="E50" r:id="rId41" display="Phoenix Contact"/>
-    <hyperlink ref="F50" r:id="rId42" display="1725672"/>
-    <hyperlink ref="E51" r:id="rId43" display="Phoenix Contact"/>
-    <hyperlink ref="E52" r:id="rId44" display="KEMET"/>
-    <hyperlink ref="G52" r:id="rId45" display="264-4141"/>
-    <hyperlink ref="F54" r:id="rId46" display="WCR0805-220KFI"/>
-    <hyperlink ref="G54" r:id="rId47" display="1099818"/>
-    <hyperlink ref="E56" r:id="rId48" display="Vishay"/>
-    <hyperlink ref="G56" r:id="rId49" display="679-1557"/>
-    <hyperlink ref="E57" r:id="rId50" display="TE Connectivity"/>
-    <hyperlink ref="G57" r:id="rId51" display="223-0562"/>
-    <hyperlink ref="E58" r:id="rId52" display="Vishay"/>
-    <hyperlink ref="F58" r:id="rId53" display="CRCW08055K00FKTA"/>
-    <hyperlink ref="G58" r:id="rId54" display="1835558"/>
+    <hyperlink ref="G12" r:id="rId4" display="1749318"/>
+    <hyperlink ref="G13" r:id="rId5" display="9886117"/>
+    <hyperlink ref="E15" r:id="rId6" display="NXP"/>
+    <hyperlink ref="F17" r:id="rId7" display="MMSZ4678T1G"/>
+    <hyperlink ref="G17" r:id="rId8" display="1459115"/>
+    <hyperlink ref="G18" r:id="rId9" display="9943641"/>
+    <hyperlink ref="G19" r:id="rId10" display="2289092"/>
+    <hyperlink ref="E20" r:id="rId11" display=" TE CONNECTIVITY / AMP"/>
+    <hyperlink ref="E23" r:id="rId12" display="STMicroelectronics"/>
+    <hyperlink ref="G23" r:id="rId13" display="314-1817"/>
+    <hyperlink ref="F25" r:id="rId14" display="CRCW060324K3FKEA"/>
+    <hyperlink ref="G25" r:id="rId15" display="2138446"/>
+    <hyperlink ref="F26" r:id="rId16" display="ERJP03F1152V"/>
+    <hyperlink ref="G26" r:id="rId17" display="2311932RL"/>
+    <hyperlink ref="F27" r:id="rId18" display="CRCW060343K2FKEA"/>
+    <hyperlink ref="G27" r:id="rId19" display="1469810"/>
+    <hyperlink ref="F28" r:id="rId20" display="CRCW0603143KFKEA"/>
+    <hyperlink ref="E30" r:id="rId21" display="Panasonic"/>
+    <hyperlink ref="E31" r:id="rId22" display="Vishay"/>
+    <hyperlink ref="G31" r:id="rId23" display="820-6745"/>
+    <hyperlink ref="E32" r:id="rId24" display="Vishay"/>
+    <hyperlink ref="G34" r:id="rId25" display="679-0419"/>
+    <hyperlink ref="G35" r:id="rId26" display="213-2143"/>
+    <hyperlink ref="G36" r:id="rId27" display="213-2266"/>
+    <hyperlink ref="E38" r:id="rId28" display="Vishay"/>
+    <hyperlink ref="G38" r:id="rId29" display="678-9926"/>
+    <hyperlink ref="G39" r:id="rId30" display="740-8805"/>
+    <hyperlink ref="G40" r:id="rId31" display="740-8877"/>
+    <hyperlink ref="G41" r:id="rId32" display="679-0251"/>
+    <hyperlink ref="G42" r:id="rId33" display="679-0689"/>
+    <hyperlink ref="G43" r:id="rId34" display="678-9960"/>
+    <hyperlink ref="G44" r:id="rId35" display="678-9822"/>
+    <hyperlink ref="E45" r:id="rId36" display="KNITTER-SWITCH"/>
+    <hyperlink ref="E46" r:id="rId37" display="TE Connectivity"/>
+    <hyperlink ref="I46" r:id="rId38" display="http://fr.rs-online.com/web/p/embases-de-circuit-imprime/4958486/"/>
+    <hyperlink ref="F47" r:id="rId39" display="LM317MDCYRG3"/>
+    <hyperlink ref="G47" r:id="rId40" display="1640686"/>
+    <hyperlink ref="E48" r:id="rId41" display="Phoenix Contact"/>
+    <hyperlink ref="E49" r:id="rId42" display="Phoenix Contact"/>
+    <hyperlink ref="E50" r:id="rId43" display="Phoenix Contact"/>
+    <hyperlink ref="F50" r:id="rId44" display="1725672"/>
+    <hyperlink ref="E51" r:id="rId45" display="Phoenix Contact"/>
+    <hyperlink ref="E52" r:id="rId46" display="KEMET"/>
+    <hyperlink ref="G52" r:id="rId47" display="264-4141"/>
+    <hyperlink ref="F54" r:id="rId48" display="WCR0805-220KFI"/>
+    <hyperlink ref="G54" r:id="rId49" display="1099818"/>
+    <hyperlink ref="E56" r:id="rId50" display="Vishay"/>
+    <hyperlink ref="E57" r:id="rId51" display="TE Connectivity"/>
+    <hyperlink ref="G57" r:id="rId52" display="223-0562"/>
+    <hyperlink ref="E58" r:id="rId53" display="Vishay Dale "/>
+    <hyperlink ref="F58" r:id="rId54" display="CRCW08055K00FKTA"/>
+    <hyperlink ref="G58" r:id="rId55" display="1835558"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2762,7 +2753,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.89795918367347"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2788,7 +2779,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.89795918367347"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>